<commit_message>
fix: the SOP form of const nodes
</commit_message>
<xml_diff>
--- a/single-selection-result.xlsx
+++ b/single-selection-result.xlsx
@@ -89,11 +89,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,118 +111,16 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCE181E"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFCE181E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -229,23 +128,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -269,25 +153,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -296,7 +163,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,96 +171,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FFCE181E"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -405,7 +191,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -693,54 +479,54 @@
       <c r="B6" s="1" t="n">
         <v>629</v>
       </c>
-      <c r="C6" s="4" t="n">
-        <v>1642</v>
+      <c r="C6" s="1" t="n">
+        <v>1615</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>1631</v>
+        <v>1600</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>8.145</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>1629</v>
+        <v>1600</v>
       </c>
       <c r="G6" s="3" t="n">
         <v>8.019</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>1620</v>
+        <v>1600</v>
       </c>
       <c r="I6" s="3" t="n">
         <v>8.408</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>1591</v>
+        <v>1579</v>
       </c>
       <c r="K6" s="3" t="n">
         <v>8.619</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>1591</v>
+        <v>1579</v>
       </c>
       <c r="M6" s="3" t="n">
         <v>8.565</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>1540</v>
+        <v>1523</v>
       </c>
       <c r="O6" s="3" t="n">
         <v>9.909</v>
       </c>
       <c r="P6" s="3" t="n">
-        <v>1500</v>
+        <v>1483</v>
       </c>
       <c r="Q6" s="1" t="n">
         <v>11.302</v>
       </c>
       <c r="R6" s="1" t="n">
         <f aca="false">(D6+F6+H6+J6+L6+N6+P6)/7/C6</f>
-        <v>0.965895249695493</v>
+        <v>0.969836355594869</v>
       </c>
       <c r="S6" s="1" t="n">
         <f aca="false">(E6+G6+I6+K6+M6+O6+Q6)/7</f>
@@ -1241,7 +1027,7 @@
       </c>
       <c r="R15" s="1" t="n">
         <f aca="false">(R3+R4+R5+R6+R7+R8+R9+R10+R11+R12+R13+R14)/12</f>
-        <v>0.778137632651811</v>
+        <v>0.778466058143426</v>
       </c>
       <c r="S15" s="1" t="n">
         <f aca="false">(S3+S4+S5+S6+S7+S8+S9+S10+S11+S12+S13+S14)/12</f>

</xml_diff>

<commit_message>
test: new synthesis script
</commit_message>
<xml_diff>
--- a/single-selection-result.xlsx
+++ b/single-selection-result.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="su" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="wu" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="20">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -89,7 +90,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -110,6 +111,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCE181E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,7 +162,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,6 +179,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -180,6 +192,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -190,8 +262,8 @@
   </sheetPr>
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -473,62 +545,62 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="4" t="n">
         <v>629</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="4" t="n">
         <v>1615</v>
       </c>
-      <c r="D6" s="3" t="n">
-        <v>1600</v>
-      </c>
-      <c r="E6" s="3" t="n">
+      <c r="D6" s="4" t="n">
+        <v>1615</v>
+      </c>
+      <c r="E6" s="4" t="n">
         <v>8.145</v>
       </c>
-      <c r="F6" s="3" t="n">
-        <v>1600</v>
-      </c>
-      <c r="G6" s="3" t="n">
+      <c r="F6" s="4" t="n">
+        <v>1607</v>
+      </c>
+      <c r="G6" s="4" t="n">
         <v>8.019</v>
       </c>
-      <c r="H6" s="3" t="n">
-        <v>1600</v>
-      </c>
-      <c r="I6" s="3" t="n">
+      <c r="H6" s="4" t="n">
+        <v>1601</v>
+      </c>
+      <c r="I6" s="4" t="n">
         <v>8.408</v>
       </c>
-      <c r="J6" s="3" t="n">
-        <v>1579</v>
-      </c>
-      <c r="K6" s="3" t="n">
+      <c r="J6" s="4" t="n">
+        <v>1576</v>
+      </c>
+      <c r="K6" s="4" t="n">
         <v>8.619</v>
       </c>
-      <c r="L6" s="3" t="n">
-        <v>1579</v>
-      </c>
-      <c r="M6" s="3" t="n">
+      <c r="L6" s="4" t="n">
+        <v>1576</v>
+      </c>
+      <c r="M6" s="4" t="n">
         <v>8.565</v>
       </c>
-      <c r="N6" s="3" t="n">
+      <c r="N6" s="4" t="n">
         <v>1523</v>
       </c>
-      <c r="O6" s="3" t="n">
+      <c r="O6" s="4" t="n">
         <v>9.909</v>
       </c>
-      <c r="P6" s="3" t="n">
-        <v>1483</v>
-      </c>
-      <c r="Q6" s="1" t="n">
+      <c r="P6" s="4" t="n">
+        <v>1480</v>
+      </c>
+      <c r="Q6" s="4" t="n">
         <v>11.302</v>
       </c>
-      <c r="R6" s="1" t="n">
+      <c r="R6" s="4" t="n">
         <f aca="false">(D6+F6+H6+J6+L6+N6+P6)/7/C6</f>
-        <v>0.969836355594869</v>
-      </c>
-      <c r="S6" s="1" t="n">
+        <v>0.971074745687749</v>
+      </c>
+      <c r="S6" s="4" t="n">
         <f aca="false">(E6+G6+I6+K6+M6+O6+Q6)/7</f>
         <v>8.99528571428571</v>
       </c>
@@ -1027,7 +1099,7 @@
       </c>
       <c r="R15" s="1" t="n">
         <f aca="false">(R3+R4+R5+R6+R7+R8+R9+R10+R11+R12+R13+R14)/12</f>
-        <v>0.778466058143426</v>
+        <v>0.778569257317832</v>
       </c>
       <c r="S15" s="1" t="n">
         <f aca="false">(S3+S4+S5+S6+S7+S8+S9+S10+S11+S12+S13+S14)/12</f>
@@ -1052,4 +1124,515 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:S15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>357</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>599</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>880</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1153</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1434</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>629</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>1615</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>1615</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>52</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>1596</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>109</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>1582</v>
+      </c>
+      <c r="I6" s="4" t="n">
+        <v>139</v>
+      </c>
+      <c r="J6" s="4" t="n">
+        <v>1568</v>
+      </c>
+      <c r="K6" s="4" t="n">
+        <v>208</v>
+      </c>
+      <c r="L6" s="4" t="n">
+        <v>1562</v>
+      </c>
+      <c r="M6" s="4" t="n">
+        <v>230</v>
+      </c>
+      <c r="N6" s="4" t="n">
+        <v>1528</v>
+      </c>
+      <c r="O6" s="4" t="n">
+        <v>563</v>
+      </c>
+      <c r="P6" s="4" t="n">
+        <v>1487</v>
+      </c>
+      <c r="Q6" s="4" t="n">
+        <v>480</v>
+      </c>
+      <c r="R6" s="4" t="n">
+        <f aca="false">(D6+F6+H6+J6+L6+N6+P6)/7/C6</f>
+        <v>0.967536488279522</v>
+      </c>
+      <c r="S6" s="4" t="n">
+        <f aca="false">(E6+G6+I6+K6+M6+O6+Q6)/7</f>
+        <v>254.428571428571</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>893</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>2432</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>1087</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>2759</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>730</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>2740</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>691</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>303</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1063</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>345</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>1128</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>436</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>1276</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>382</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>1104</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test: add manual test
</commit_message>
<xml_diff>
--- a/single-selection-result.xlsx
+++ b/single-selection-result.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="su" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="wu" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="22">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -29,6 +30,57 @@
     <t xml:space="preserve">#nodes</t>
   </si>
   <si>
+    <t xml:space="preserve">Ori Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c880</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c1908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c2670</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c3540</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5315</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c7552</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alu4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RCA32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLA32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KSA32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUL8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WTM8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average</t>
+  </si>
+  <si>
     <t xml:space="preserve">Original area</t>
   </si>
   <si>
@@ -36,59 +88,16 @@
   </si>
   <si>
     <t xml:space="preserve">Average time/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c880</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c1908</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c2670</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c3540</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c5315</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c7552</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alu4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RCA32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLA32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KSA32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUL8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WTM8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">average</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -162,7 +171,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,7 +180,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -179,7 +192,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -262,13 +299,27 @@
   </sheetPr>
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="18" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -282,88 +333,88 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="n">
+      <c r="D1" s="3" t="n">
         <v>0.001</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="n">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="n">
         <v>0.003</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="n">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="n">
         <v>0.005</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="n">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="n">
         <v>0.008</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="n">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="n">
         <v>0.01</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="n">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="n">
         <v>0.03</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2" t="n">
+      <c r="O1" s="3"/>
+      <c r="P1" s="3" t="n">
         <v>0.05</v>
       </c>
-      <c r="Q1" s="2"/>
+      <c r="Q1" s="3"/>
       <c r="R1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="M2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="O2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>6</v>
+      <c r="Q2" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>357</v>
@@ -371,60 +422,60 @@
       <c r="C3" s="1" t="n">
         <v>599</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="4" t="n">
         <v>529</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="5" t="n">
         <v>1.757</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <v>524</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="G3" s="2" t="n">
         <v>1.871</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="4" t="n">
         <v>517</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="5" t="n">
         <v>2.119</v>
       </c>
-      <c r="J3" s="3" t="n">
+      <c r="J3" s="4" t="n">
         <v>517</v>
       </c>
-      <c r="K3" s="3" t="n">
+      <c r="K3" s="5" t="n">
         <v>2.158</v>
       </c>
-      <c r="L3" s="3" t="n">
+      <c r="L3" s="4" t="n">
         <v>497</v>
       </c>
-      <c r="M3" s="3" t="n">
+      <c r="M3" s="5" t="n">
         <v>2.171</v>
       </c>
-      <c r="N3" s="3" t="n">
+      <c r="N3" s="4" t="n">
         <v>497</v>
       </c>
-      <c r="O3" s="3" t="n">
+      <c r="O3" s="5" t="n">
         <v>2.327</v>
       </c>
-      <c r="P3" s="3" t="n">
+      <c r="P3" s="4" t="n">
         <v>493</v>
       </c>
-      <c r="Q3" s="1" t="n">
+      <c r="Q3" s="2" t="n">
         <v>2.43</v>
       </c>
-      <c r="R3" s="1" t="n">
+      <c r="R3" s="6" t="n">
         <f aca="false">(D3+F3+H3+J3+L3+N3+P3)/7/C3</f>
         <v>0.85237300262342</v>
       </c>
-      <c r="S3" s="1" t="n">
+      <c r="S3" s="2" t="n">
         <f aca="false">(E3+G3+I3+K3+M3+O3+Q3)/7</f>
         <v>2.119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>880</v>
@@ -432,60 +483,60 @@
       <c r="C4" s="1" t="n">
         <v>1013</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="4" t="n">
         <v>627</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="5" t="n">
         <v>0.88</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <v>620</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="G4" s="5" t="n">
         <v>0.932</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="4" t="n">
         <v>619</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="5" t="n">
         <v>1.058</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="4" t="n">
         <v>593</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="K4" s="5" t="n">
         <v>1.197</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="L4" s="4" t="n">
         <v>579</v>
       </c>
-      <c r="M4" s="3" t="n">
+      <c r="M4" s="5" t="n">
         <v>1.268</v>
       </c>
-      <c r="N4" s="3" t="n">
+      <c r="N4" s="4" t="n">
         <v>495</v>
       </c>
-      <c r="O4" s="3" t="n">
+      <c r="O4" s="5" t="n">
         <v>1.384</v>
       </c>
-      <c r="P4" s="3" t="n">
+      <c r="P4" s="4" t="n">
         <v>279</v>
       </c>
-      <c r="Q4" s="1" t="n">
+      <c r="Q4" s="2" t="n">
         <v>9.062</v>
       </c>
-      <c r="R4" s="1" t="n">
+      <c r="R4" s="6" t="n">
         <f aca="false">(D4+F4+H4+J4+L4+N4+P4)/7/C4</f>
         <v>0.537582851501904</v>
       </c>
-      <c r="S4" s="1" t="n">
+      <c r="S4" s="2" t="n">
         <f aca="false">(E4+G4+I4+K4+M4+O4+Q4)/7</f>
         <v>2.25442857142857</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>1153</v>
@@ -493,121 +544,121 @@
       <c r="C5" s="1" t="n">
         <v>1434</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="4" t="n">
         <v>868</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="5" t="n">
         <v>51.829</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="4" t="n">
         <v>868</v>
       </c>
-      <c r="G5" s="3" t="n">
+      <c r="G5" s="5" t="n">
         <v>53.663</v>
       </c>
-      <c r="H5" s="3" t="n">
+      <c r="H5" s="4" t="n">
         <v>860</v>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="I5" s="5" t="n">
         <v>52.378</v>
       </c>
-      <c r="J5" s="3" t="n">
+      <c r="J5" s="4" t="n">
         <v>860</v>
       </c>
-      <c r="K5" s="3" t="n">
+      <c r="K5" s="5" t="n">
         <v>50.306</v>
       </c>
-      <c r="L5" s="3" t="n">
+      <c r="L5" s="4" t="n">
         <v>860</v>
       </c>
-      <c r="M5" s="3" t="n">
+      <c r="M5" s="5" t="n">
         <v>50.33</v>
       </c>
-      <c r="N5" s="3" t="n">
+      <c r="N5" s="4" t="n">
         <v>845</v>
       </c>
-      <c r="O5" s="3" t="n">
+      <c r="O5" s="5" t="n">
         <v>53.214</v>
       </c>
-      <c r="P5" s="3" t="n">
+      <c r="P5" s="4" t="n">
         <v>841</v>
       </c>
-      <c r="Q5" s="1" t="n">
+      <c r="Q5" s="2" t="n">
         <v>53.996</v>
       </c>
-      <c r="R5" s="1" t="n">
+      <c r="R5" s="6" t="n">
         <f aca="false">(D5+F5+H5+J5+L5+N5+P5)/7/C5</f>
         <v>0.597927874078502</v>
       </c>
-      <c r="S5" s="1" t="n">
+      <c r="S5" s="2" t="n">
         <f aca="false">(E5+G5+I5+K5+M5+O5+Q5)/7</f>
         <v>52.2451428571429</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="n">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="7" t="n">
         <v>629</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="7" t="n">
         <v>1615</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="7" t="n">
         <v>1615</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="8" t="n">
         <v>8.145</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F6" s="7" t="n">
         <v>1607</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="8" t="n">
         <v>8.019</v>
       </c>
-      <c r="H6" s="4" t="n">
+      <c r="H6" s="7" t="n">
         <v>1601</v>
       </c>
-      <c r="I6" s="4" t="n">
+      <c r="I6" s="8" t="n">
         <v>8.408</v>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="7" t="n">
         <v>1576</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="8" t="n">
         <v>8.619</v>
       </c>
-      <c r="L6" s="4" t="n">
+      <c r="L6" s="7" t="n">
         <v>1576</v>
       </c>
-      <c r="M6" s="4" t="n">
+      <c r="M6" s="8" t="n">
         <v>8.565</v>
       </c>
-      <c r="N6" s="4" t="n">
+      <c r="N6" s="7" t="n">
         <v>1523</v>
       </c>
-      <c r="O6" s="4" t="n">
+      <c r="O6" s="8" t="n">
         <v>9.909</v>
       </c>
-      <c r="P6" s="4" t="n">
+      <c r="P6" s="7" t="n">
         <v>1480</v>
       </c>
-      <c r="Q6" s="4" t="n">
+      <c r="Q6" s="8" t="n">
         <v>11.302</v>
       </c>
-      <c r="R6" s="4" t="n">
+      <c r="R6" s="9" t="n">
         <f aca="false">(D6+F6+H6+J6+L6+N6+P6)/7/C6</f>
         <v>0.971074745687749</v>
       </c>
-      <c r="S6" s="4" t="n">
+      <c r="S6" s="8" t="n">
         <f aca="false">(E6+G6+I6+K6+M6+O6+Q6)/7</f>
         <v>8.99528571428571</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>893</v>
@@ -615,60 +666,60 @@
       <c r="C7" s="1" t="n">
         <v>2432</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="4" t="n">
         <v>2303</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="5" t="n">
         <v>50.534</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <v>2303</v>
       </c>
-      <c r="G7" s="3" t="n">
+      <c r="G7" s="5" t="n">
         <v>50.084</v>
       </c>
-      <c r="H7" s="3" t="n">
+      <c r="H7" s="4" t="n">
         <v>2297</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="5" t="n">
         <v>50.703</v>
       </c>
-      <c r="J7" s="3" t="n">
+      <c r="J7" s="4" t="n">
         <v>2297</v>
       </c>
-      <c r="K7" s="3" t="n">
+      <c r="K7" s="5" t="n">
         <v>51.86</v>
       </c>
-      <c r="L7" s="3" t="n">
+      <c r="L7" s="4" t="n">
         <v>2291</v>
       </c>
-      <c r="M7" s="3" t="n">
+      <c r="M7" s="5" t="n">
         <v>53.009</v>
       </c>
-      <c r="N7" s="3" t="n">
+      <c r="N7" s="4" t="n">
         <v>2282</v>
       </c>
-      <c r="O7" s="3" t="n">
+      <c r="O7" s="5" t="n">
         <v>53.422</v>
       </c>
-      <c r="P7" s="3" t="n">
+      <c r="P7" s="4" t="n">
         <v>2282</v>
       </c>
-      <c r="Q7" s="1" t="n">
+      <c r="Q7" s="2" t="n">
         <v>55.985</v>
       </c>
-      <c r="R7" s="1" t="n">
+      <c r="R7" s="6" t="n">
         <f aca="false">(D7+F7+H7+J7+L7+N7+P7)/7/C7</f>
         <v>0.943080357142857</v>
       </c>
-      <c r="S7" s="1" t="n">
+      <c r="S7" s="2" t="n">
         <f aca="false">(E7+G7+I7+K7+M7+O7+Q7)/7</f>
         <v>52.2281428571429</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1087</v>
@@ -676,60 +727,60 @@
       <c r="C8" s="1" t="n">
         <v>2759</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="4" t="n">
         <v>2403</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="5" t="n">
         <v>12.194</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="4" t="n">
         <v>2390</v>
       </c>
-      <c r="G8" s="3" t="n">
+      <c r="G8" s="5" t="n">
         <v>19.289</v>
       </c>
-      <c r="H8" s="3" t="n">
+      <c r="H8" s="4" t="n">
         <v>2374</v>
       </c>
-      <c r="I8" s="3" t="n">
+      <c r="I8" s="5" t="n">
         <v>19.575</v>
       </c>
-      <c r="J8" s="3" t="n">
+      <c r="J8" s="4" t="n">
         <v>2351</v>
       </c>
-      <c r="K8" s="3" t="n">
+      <c r="K8" s="5" t="n">
         <v>21.963</v>
       </c>
-      <c r="L8" s="3" t="n">
+      <c r="L8" s="4" t="n">
         <v>2351</v>
       </c>
-      <c r="M8" s="3" t="n">
+      <c r="M8" s="5" t="n">
         <v>21.509</v>
       </c>
-      <c r="N8" s="3" t="n">
+      <c r="N8" s="4" t="n">
         <v>2339</v>
       </c>
-      <c r="O8" s="3" t="n">
+      <c r="O8" s="5" t="n">
         <v>22.764</v>
       </c>
-      <c r="P8" s="3" t="n">
+      <c r="P8" s="4" t="n">
         <v>2331</v>
       </c>
-      <c r="Q8" s="3" t="n">
+      <c r="Q8" s="5" t="n">
         <v>22.83</v>
       </c>
-      <c r="R8" s="1" t="n">
+      <c r="R8" s="6" t="n">
         <f aca="false">(D8+F8+H8+J8+L8+N8+P8)/7/C8</f>
         <v>0.856366178221923</v>
       </c>
-      <c r="S8" s="1" t="n">
+      <c r="S8" s="2" t="n">
         <f aca="false">(E8+G8+I8+K8+M8+O8+Q8)/7</f>
         <v>20.0177142857143</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>730</v>
@@ -737,60 +788,60 @@
       <c r="C9" s="1" t="n">
         <v>2740</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="4" t="n">
         <v>2239</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="5" t="n">
         <v>17.509</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="4" t="n">
         <v>2163</v>
       </c>
-      <c r="G9" s="3" t="n">
+      <c r="G9" s="5" t="n">
         <v>19.644</v>
       </c>
-      <c r="H9" s="3" t="n">
+      <c r="H9" s="4" t="n">
         <v>2150</v>
       </c>
-      <c r="I9" s="3" t="n">
+      <c r="I9" s="5" t="n">
         <v>21.322</v>
       </c>
-      <c r="J9" s="3" t="n">
+      <c r="J9" s="4" t="n">
         <v>2036</v>
       </c>
-      <c r="K9" s="3" t="n">
+      <c r="K9" s="5" t="n">
         <v>24.402</v>
       </c>
-      <c r="L9" s="3" t="n">
+      <c r="L9" s="4" t="n">
         <v>1941</v>
       </c>
-      <c r="M9" s="3" t="n">
+      <c r="M9" s="5" t="n">
         <v>25.217</v>
       </c>
-      <c r="N9" s="3" t="n">
+      <c r="N9" s="4" t="n">
         <v>1659</v>
       </c>
-      <c r="O9" s="3" t="n">
+      <c r="O9" s="5" t="n">
         <v>30.55</v>
       </c>
-      <c r="P9" s="3" t="n">
+      <c r="P9" s="4" t="n">
         <v>1611</v>
       </c>
-      <c r="Q9" s="3" t="n">
+      <c r="Q9" s="5" t="n">
         <v>32.986</v>
       </c>
-      <c r="R9" s="3" t="n">
+      <c r="R9" s="10" t="n">
         <f aca="false">(D9+F9+H9+J9+L9+N9+P9)/7/C9</f>
         <v>0.719447340980188</v>
       </c>
-      <c r="S9" s="3" t="n">
+      <c r="S9" s="5" t="n">
         <f aca="false">(E9+G9+I9+K9+M9+O9+Q9)/7</f>
         <v>24.5185714285714</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>202</v>
@@ -798,60 +849,60 @@
       <c r="C10" s="1" t="n">
         <v>691</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="4" t="n">
         <v>570</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="5" t="n">
         <v>1.095</v>
       </c>
-      <c r="F10" s="3" t="n">
+      <c r="F10" s="4" t="n">
         <v>557</v>
       </c>
-      <c r="G10" s="3" t="n">
+      <c r="G10" s="5" t="n">
         <v>1.227</v>
       </c>
-      <c r="H10" s="3" t="n">
+      <c r="H10" s="4" t="n">
         <v>557</v>
       </c>
-      <c r="I10" s="3" t="n">
+      <c r="I10" s="5" t="n">
         <v>1.385</v>
       </c>
-      <c r="J10" s="3" t="n">
+      <c r="J10" s="4" t="n">
         <v>557</v>
       </c>
-      <c r="K10" s="3" t="n">
+      <c r="K10" s="5" t="n">
         <v>1.367</v>
       </c>
-      <c r="L10" s="3" t="n">
+      <c r="L10" s="4" t="n">
         <v>557</v>
       </c>
-      <c r="M10" s="3" t="n">
+      <c r="M10" s="5" t="n">
         <v>1.365</v>
       </c>
-      <c r="N10" s="3" t="n">
+      <c r="N10" s="4" t="n">
         <v>557</v>
       </c>
-      <c r="O10" s="3" t="n">
+      <c r="O10" s="5" t="n">
         <v>1.401</v>
       </c>
-      <c r="P10" s="3" t="n">
+      <c r="P10" s="4" t="n">
         <v>557</v>
       </c>
-      <c r="Q10" s="3" t="n">
+      <c r="Q10" s="5" t="n">
         <v>1.509</v>
       </c>
-      <c r="R10" s="3" t="n">
+      <c r="R10" s="10" t="n">
         <f aca="false">(D10+F10+H10+J10+L10+N10+P10)/7/C10</f>
         <v>0.808765763903246</v>
       </c>
-      <c r="S10" s="3" t="n">
+      <c r="S10" s="5" t="n">
         <f aca="false">(E10+G10+I10+K10+M10+O10+Q10)/7</f>
         <v>1.33557142857143</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>303</v>
@@ -859,60 +910,60 @@
       <c r="C11" s="1" t="n">
         <v>1063</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="4" t="n">
         <v>689</v>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="5" t="n">
         <v>3.183</v>
       </c>
-      <c r="F11" s="3" t="n">
+      <c r="F11" s="4" t="n">
         <v>689</v>
       </c>
-      <c r="G11" s="3" t="n">
+      <c r="G11" s="5" t="n">
         <v>3.161</v>
       </c>
-      <c r="H11" s="3" t="n">
+      <c r="H11" s="4" t="n">
         <v>656</v>
       </c>
-      <c r="I11" s="3" t="n">
+      <c r="I11" s="5" t="n">
         <v>3.481</v>
       </c>
-      <c r="J11" s="3" t="n">
+      <c r="J11" s="4" t="n">
         <v>656</v>
       </c>
-      <c r="K11" s="3" t="n">
+      <c r="K11" s="5" t="n">
         <v>3.457</v>
       </c>
-      <c r="L11" s="3" t="n">
+      <c r="L11" s="4" t="n">
         <v>656</v>
       </c>
-      <c r="M11" s="3" t="n">
+      <c r="M11" s="5" t="n">
         <v>3.799</v>
       </c>
-      <c r="N11" s="3" t="n">
+      <c r="N11" s="4" t="n">
         <v>645</v>
       </c>
-      <c r="O11" s="3" t="n">
+      <c r="O11" s="5" t="n">
         <v>3.985</v>
       </c>
-      <c r="P11" s="3" t="n">
+      <c r="P11" s="4" t="n">
         <v>645</v>
       </c>
-      <c r="Q11" s="3" t="n">
+      <c r="Q11" s="5" t="n">
         <v>4.071</v>
       </c>
-      <c r="R11" s="3" t="n">
+      <c r="R11" s="10" t="n">
         <f aca="false">(D11+F11+H11+J11+L11+N11+P11)/7/C11</f>
         <v>0.623034538368499</v>
       </c>
-      <c r="S11" s="3" t="n">
+      <c r="S11" s="5" t="n">
         <f aca="false">(E11+G11+I11+K11+M11+O11+Q11)/7</f>
         <v>3.591</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>345</v>
@@ -920,60 +971,60 @@
       <c r="C12" s="1" t="n">
         <v>1128</v>
       </c>
-      <c r="D12" s="3" t="n">
+      <c r="D12" s="4" t="n">
         <v>911</v>
       </c>
-      <c r="E12" s="3" t="n">
+      <c r="E12" s="5" t="n">
         <v>3.662</v>
       </c>
-      <c r="F12" s="3" t="n">
+      <c r="F12" s="4" t="n">
         <v>906</v>
       </c>
-      <c r="G12" s="3" t="n">
+      <c r="G12" s="5" t="n">
         <v>3.883</v>
       </c>
-      <c r="H12" s="3" t="n">
+      <c r="H12" s="4" t="n">
         <v>892</v>
       </c>
-      <c r="I12" s="3" t="n">
+      <c r="I12" s="5" t="n">
         <v>4.071</v>
       </c>
-      <c r="J12" s="3" t="n">
+      <c r="J12" s="4" t="n">
         <v>859</v>
       </c>
-      <c r="K12" s="3" t="n">
+      <c r="K12" s="5" t="n">
         <v>4.361</v>
       </c>
-      <c r="L12" s="3" t="n">
+      <c r="L12" s="4" t="n">
         <v>840</v>
       </c>
-      <c r="M12" s="3" t="n">
+      <c r="M12" s="5" t="n">
         <v>4.386</v>
       </c>
-      <c r="N12" s="3" t="n">
+      <c r="N12" s="4" t="n">
         <v>770</v>
       </c>
-      <c r="O12" s="3" t="n">
+      <c r="O12" s="5" t="n">
         <v>7.767</v>
       </c>
-      <c r="P12" s="3" t="n">
+      <c r="P12" s="4" t="n">
         <v>755</v>
       </c>
-      <c r="Q12" s="3" t="n">
+      <c r="Q12" s="5" t="n">
         <v>7.818</v>
       </c>
-      <c r="R12" s="3" t="n">
+      <c r="R12" s="10" t="n">
         <f aca="false">(D12+F12+H12+J12+L12+N12+P12)/7/C12</f>
         <v>0.751393110435664</v>
       </c>
-      <c r="S12" s="3" t="n">
+      <c r="S12" s="5" t="n">
         <f aca="false">(E12+G12+I12+K12+M12+O12+Q12)/7</f>
         <v>5.13542857142857</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>436</v>
@@ -981,60 +1032,60 @@
       <c r="C13" s="1" t="n">
         <v>1276</v>
       </c>
-      <c r="D13" s="3" t="n">
+      <c r="D13" s="4" t="n">
         <v>1025</v>
       </c>
-      <c r="E13" s="3" t="n">
+      <c r="E13" s="5" t="n">
         <v>2.105</v>
       </c>
-      <c r="F13" s="3" t="n">
+      <c r="F13" s="4" t="n">
         <v>1025</v>
       </c>
-      <c r="G13" s="3" t="n">
+      <c r="G13" s="5" t="n">
         <v>2.02</v>
       </c>
-      <c r="H13" s="3" t="n">
+      <c r="H13" s="4" t="n">
         <v>1025</v>
       </c>
-      <c r="I13" s="3" t="n">
+      <c r="I13" s="5" t="n">
         <v>2.013</v>
       </c>
-      <c r="J13" s="3" t="n">
+      <c r="J13" s="4" t="n">
         <v>1025</v>
       </c>
-      <c r="K13" s="3" t="n">
+      <c r="K13" s="5" t="n">
         <v>2.18</v>
       </c>
-      <c r="L13" s="3" t="n">
+      <c r="L13" s="4" t="n">
         <v>1025</v>
       </c>
-      <c r="M13" s="3" t="n">
+      <c r="M13" s="5" t="n">
         <v>2.148</v>
       </c>
-      <c r="N13" s="3" t="n">
+      <c r="N13" s="4" t="n">
         <v>1025</v>
       </c>
-      <c r="O13" s="3" t="n">
+      <c r="O13" s="5" t="n">
         <v>2.204</v>
       </c>
-      <c r="P13" s="3" t="n">
+      <c r="P13" s="4" t="n">
         <v>1025</v>
       </c>
-      <c r="Q13" s="3" t="n">
+      <c r="Q13" s="5" t="n">
         <v>2.23</v>
       </c>
-      <c r="R13" s="3" t="n">
+      <c r="R13" s="10" t="n">
         <f aca="false">(D13+F13+H13+J13+L13+N13+P13)/7/C13</f>
         <v>0.803291536050157</v>
       </c>
-      <c r="S13" s="3" t="n">
+      <c r="S13" s="5" t="n">
         <f aca="false">(E13+G13+I13+K13+M13+O13+Q13)/7</f>
         <v>2.12857142857143</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>382</v>
@@ -1042,66 +1093,66 @@
       <c r="C14" s="1" t="n">
         <v>1104</v>
       </c>
-      <c r="D14" s="3" t="n">
+      <c r="D14" s="4" t="n">
         <v>971</v>
       </c>
-      <c r="E14" s="3" t="n">
+      <c r="E14" s="5" t="n">
         <v>3.221</v>
       </c>
-      <c r="F14" s="3" t="n">
+      <c r="F14" s="4" t="n">
         <v>971</v>
       </c>
-      <c r="G14" s="3" t="n">
+      <c r="G14" s="5" t="n">
         <v>3.286</v>
       </c>
-      <c r="H14" s="3" t="n">
+      <c r="H14" s="4" t="n">
         <v>971</v>
       </c>
-      <c r="I14" s="3" t="n">
+      <c r="I14" s="5" t="n">
         <v>3.365</v>
       </c>
-      <c r="J14" s="3" t="n">
+      <c r="J14" s="4" t="n">
         <v>971</v>
       </c>
-      <c r="K14" s="3" t="n">
+      <c r="K14" s="5" t="n">
         <v>3.645</v>
       </c>
-      <c r="L14" s="3" t="n">
+      <c r="L14" s="4" t="n">
         <v>971</v>
       </c>
-      <c r="M14" s="3" t="n">
+      <c r="M14" s="5" t="n">
         <v>3.6</v>
       </c>
-      <c r="N14" s="3" t="n">
+      <c r="N14" s="4" t="n">
         <v>971</v>
       </c>
-      <c r="O14" s="3" t="n">
+      <c r="O14" s="5" t="n">
         <v>3.737</v>
       </c>
-      <c r="P14" s="3" t="n">
+      <c r="P14" s="4" t="n">
         <v>963</v>
       </c>
-      <c r="Q14" s="3" t="n">
+      <c r="Q14" s="5" t="n">
         <v>3.896</v>
       </c>
-      <c r="R14" s="3" t="n">
+      <c r="R14" s="10" t="n">
         <f aca="false">(D14+F14+H14+J14+L14+N14+P14)/7/C14</f>
         <v>0.878493788819876</v>
       </c>
-      <c r="S14" s="3" t="n">
+      <c r="S14" s="5" t="n">
         <f aca="false">(E14+G14+I14+K14+M14+O14+Q14)/7</f>
         <v>3.53571428571429</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R15" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="R15" s="6" t="n">
         <f aca="false">(R3+R4+R5+R6+R7+R8+R9+R10+R11+R12+R13+R14)/12</f>
         <v>0.778569257317832</v>
       </c>
-      <c r="S15" s="1" t="n">
+      <c r="S15" s="2" t="n">
         <f aca="false">(S3+S4+S5+S6+S7+S8+S9+S10+S11+S12+S13+S14)/12</f>
         <v>14.8420476190476</v>
       </c>
@@ -1133,8 +1184,8 @@
   </sheetPr>
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q11" activeCellId="0" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1150,95 +1201,95 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="D1" s="11" t="n">
         <v>0.001</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="n">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="n">
         <v>0.003</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="n">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11" t="n">
         <v>0.005</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="n">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11" t="n">
         <v>0.008</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="n">
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="n">
         <v>0.01</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="n">
+      <c r="M1" s="11"/>
+      <c r="N1" s="11" t="n">
         <v>0.03</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2" t="n">
+      <c r="O1" s="11"/>
+      <c r="P1" s="11" t="n">
         <v>0.05</v>
       </c>
-      <c r="Q1" s="2"/>
+      <c r="Q1" s="11"/>
       <c r="R1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>4</v>
+        <v>20</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="M2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="O2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>6</v>
+      <c r="Q2" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>357</v>
@@ -1246,26 +1297,26 @@
       <c r="C3" s="1" t="n">
         <v>599</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>880</v>
@@ -1273,26 +1324,26 @@
       <c r="C4" s="1" t="n">
         <v>1013</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>1153</v>
@@ -1300,87 +1351,87 @@
       <c r="C5" s="1" t="n">
         <v>1434</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="n">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="7" t="n">
         <v>629</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="7" t="n">
         <v>1615</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="7" t="n">
         <v>1615</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="7" t="n">
         <v>52</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F6" s="7" t="n">
         <v>1596</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="7" t="n">
         <v>109</v>
       </c>
-      <c r="H6" s="4" t="n">
+      <c r="H6" s="7" t="n">
         <v>1582</v>
       </c>
-      <c r="I6" s="4" t="n">
+      <c r="I6" s="7" t="n">
         <v>139</v>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="7" t="n">
         <v>1568</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="7" t="n">
         <v>208</v>
       </c>
-      <c r="L6" s="4" t="n">
+      <c r="L6" s="7" t="n">
         <v>1562</v>
       </c>
-      <c r="M6" s="4" t="n">
+      <c r="M6" s="7" t="n">
         <v>230</v>
       </c>
-      <c r="N6" s="4" t="n">
+      <c r="N6" s="7" t="n">
         <v>1528</v>
       </c>
-      <c r="O6" s="4" t="n">
+      <c r="O6" s="7" t="n">
         <v>563</v>
       </c>
-      <c r="P6" s="4" t="n">
+      <c r="P6" s="7" t="n">
         <v>1487</v>
       </c>
-      <c r="Q6" s="4" t="n">
+      <c r="Q6" s="7" t="n">
         <v>480</v>
       </c>
-      <c r="R6" s="4" t="n">
+      <c r="R6" s="7" t="n">
         <f aca="false">(D6+F6+H6+J6+L6+N6+P6)/7/C6</f>
         <v>0.967536488279522</v>
       </c>
-      <c r="S6" s="4" t="n">
+      <c r="S6" s="7" t="n">
         <f aca="false">(E6+G6+I6+K6+M6+O6+Q6)/7</f>
         <v>254.428571428571</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>893</v>
@@ -1388,26 +1439,26 @@
       <c r="C7" s="1" t="n">
         <v>2432</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1087</v>
@@ -1415,26 +1466,26 @@
       <c r="C8" s="1" t="n">
         <v>2759</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>730</v>
@@ -1442,26 +1493,26 @@
       <c r="C9" s="1" t="n">
         <v>2740</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>202</v>
@@ -1469,26 +1520,26 @@
       <c r="C10" s="1" t="n">
         <v>691</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>303</v>
@@ -1496,26 +1547,26 @@
       <c r="C11" s="1" t="n">
         <v>1063</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>345</v>
@@ -1523,26 +1574,26 @@
       <c r="C12" s="1" t="n">
         <v>1128</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>436</v>
@@ -1550,26 +1601,26 @@
       <c r="C13" s="1" t="n">
         <v>1276</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>382</v>
@@ -1577,26 +1628,26 @@
       <c r="C14" s="1" t="n">
         <v>1104</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1635,4 +1686,103 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>0.893</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0.595</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0.662</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.966</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0.978</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0.878</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0.822</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0.827</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0.819</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>0.953</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <f aca="false">(A1+A2+A3+A4+A5+A6+A7+A8+A9+A10+A11+A12)/12</f>
+        <v>0.858583333333333</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <f aca="false">A1*A2*A3*A4*A5*A6*A7*A8*A9*A10*A11*A12</f>
+        <v>0.141153167595001</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>